<commit_message>
ADDING FINE-TUNINGv2.jsonl ALL OK
</commit_message>
<xml_diff>
--- a/SimulationManager/Training LLM/TrainingStats.xlsx
+++ b/SimulationManager/Training LLM/TrainingStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\UnityProjects\SimulationManager\Training LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8382C046-0BAD-4AC6-9254-604207F72CB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3233A-12AB-40B8-BF81-2E2364588756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{21FFF4A9-BEE3-4716-82C1-DB13693BAF4B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>MODELO</t>
   </si>
@@ -166,6 +166,39 @@
   </si>
   <si>
     <t>5.EColiSystem.cs{Dependency=Entities.WithReadOnly(parentMap).ForEach((Entity entity,int entityInQueryIndex,ref LocalTransform transform,ref EColiComponent organism)=&gt;{float maxScale=organism.MaxScale;organism.GrowthDuration=organism.DivisionInterval=organism.TimeReference*organism.SeparationThreshold;if(transform.Scale&lt;maxScale){organism.GrowthTime+=deltaTime;float t=math.clamp(organism.GrowthTime/organism.GrowthDuration,0f,1f);float initialScale=organism.IsInitialCell?maxScale:0.01f;transform.Scale=math.lerp(initialScale,maxScale,t);}if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*12345);int sign=rng.NextFloat()&lt;0.5f?1:-1;Entity child=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform childTransform=transform;childTransform.Scale=0.01f;EColiComponent childData=organism;childData.GrowthTime=0f;childData.TimeSinceLastDivision=0f;childData.HasGeneratedChild=false;childData.IsInitialCell=false;childData.Parent=entity;childData.SeparationSign=sign;float3 upDir=math.mul(transform.Rotation,new float3(0,sign,0));childTransform.Position=transform.Position+upDir*(transform.Scale*0.25f);ecb.SetComponent(entityInQueryIndex,child,childTransform);ecb.SetComponent(entityInQueryIndex,child,childData);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData parentData)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float offset=math.lerp(0f,parentData.Scale*4.9f,transform.Scale/maxScale);float3 up=math.mul(parentData.Rotation,new float3(0,organism.SeparationSign,0));transform.Position=parentData.Position+up*offset;transform.Rotation=parentData.Rotation;}else organism.Parent=Entity.Null;}}</t>
+  </si>
+  <si>
+    <t>NUEVO DESGLOSE RESPUESTA ASSISTANT</t>
+  </si>
+  <si>
+    <t>1.PrefabMaterialCreator.cs{public static class PrefabMaterialCreator{const string pF=\"Assets/Resources/Prefabs\",mF=\"Assets/Resources/PrefabsMaterials\";[MenuItem(\"Tools/Crear Prefabs y Materiales\")]public static void CreatePrefabsAndMaterials(){if(!AssetDatabase.IsValidFolder(pF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"Prefabs\");Debug.Log(\"Carpeta creada: \"+pF);}if(!AssetDatabase.IsValidFolder(mF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"PrefabsMaterials\");Debug.Log(\"Carpeta creada: \"+mF);}CPAM(\"SCerevisiae\",PrimitiveType.Sphere,new Vector3(5,5,5),new Vector3(90,0,0),0);CPAM(\"EColi\",PrimitiveType.Capsule,new Vector3(.5f,2,0.5f),new Vector3(90,0,0),1);AssetDatabase.SaveAssets();AssetDatabase.Refresh();Debug.Log(\"Prefabs y materiales creados.\");}static void CPAM(string n,PrimitiveType t,Vector3 s,Vector3 r,int c){var o=GameObject.CreatePrimitive(t);o.name=n;o.transform.rotation=Quaternion.Euler(r);o.transform.localScale=s;var col=o.GetComponent&lt;Collider&gt;();if(col!=null)Object.DestroyImmediate(col);if(c==0)o.AddComponent&lt;SphereCollider&gt;();else o.AddComponent&lt;CapsuleCollider&gt;();var sh=Shader.Find(\"Universal Render Pipeline/Lit\");if(sh==null){Debug.LogError(\"Shader URP/Lit no encontrado.\");return;}var m=new Material(sh);m.color=n==\"SCerevisiae\"?new Color(0,0,1,1):n==\"EColi\"?new Color(0,1,0,1):Color.white;AssetDatabase.CreateAsset(m,Path.Combine(mF,n+\".mat\"));AssetDatabase.SaveAssets();AssetDatabase.Refresh();o.GetComponent&lt;Renderer&gt;().sharedMaterial=m;PrefabUtility.SaveAsPrefabAsset(o,Path.Combine(pF,n+\".prefab\"));Object.DestroyImmediate(o);}}}</t>
+  </si>
+  <si>
+    <t>2.CreatePrefabsOnClick.cs{private void CrearEntidad(Vector3 p){if(currentPrefabIndex&gt;=prefabs.Count)return;var sQ=spawnerQuery.ToEntityArray(Allocator.Temp);if(currentPrefabIndex&gt;=sQ.Length){Debug.LogError($\"No se encontró spawner en índice {currentPrefabIndex}\");sQ.Dispose();return;}Entity s=sQ[currentPrefabIndex];sQ.Dispose();Entity pe=entityManager.GetComponentData&lt;PrefabEntityComponent&gt;(s).prefab;Entity e=entityManager.Instantiate(pe);float os=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Scale;quaternion or=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Rotation;float ry=UnityEngine.Random.Range(0f,360f);quaternion nr=math.mul(or,quaternion.RotateY(math.radians(ry)));float h=os*.5f;float3 ap=new float3(p.x,math.max(p.y+h,h),p.z);entityManager.SetComponentData(e,new LocalTransform{Position=ap,Rotation=nr,Scale=os});string n=prefabs[currentPrefabIndex].name;switch(n){case\"EColi\":entityManager.AddComponentData(e,new EColiComponent{TimeReference=1200f,SeparationThreshold=0.7f,MaxScale=1f,GrowthTime=0f,GrowthDuration=1200f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=1200f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;case\"SCerevisiae\":entityManager.AddComponentData(e,new SCerevisiaeComponent{TimeReference=5400f,SeparationThreshold=0.7f,MaxScale=5f,GrowthTime=0f,GrowthDuration=5400f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=5400f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;default:Debug.LogWarning($\"No hay componente ECS para '{n}'\");break;}AddPhysicsComponents(e,n,os);Debug.Log($\"Entidad '{n}' creada en {ap}\");}private void AddPhysicsComponents(Entity e,string n,float s){BlobAssetReference&lt;Unity.Physics.Collider&gt;c=default;Material m=new Material{Friction=8f,Restitution=0f};switch(n){case\"EColi\":c=Unity.Physics.CapsuleCollider.Create(new CapsuleGeometry{Vertex0=new float3(0,-s,0),Vertex1=new float3(0,s,0),Radius=0.25f},CollisionFilter.Default,m);break;case\"SCerevisiae\":c=Unity.Physics.SphereCollider.Create(new SphereGeometry{Center=float3.zero,Radius=s*0.1f},CollisionFilter.Default,m);break;default:Debug.LogWarning($\"No collider para '{n}'\");return;}entityManager.AddComponentData(e,new PhysicsCollider{Value=c});if(c.IsCreated){var mp=c.Value.MassProperties;entityManager.AddComponentData(e,PhysicsMass.CreateDynamic(mp,1f));}entityManager.AddComponentData(e,new PhysicsVelocity{Linear=float3.zero,Angular=float3.zero});entityManager.AddComponentData(e,new PhysicsGravityFactor{Value=1f});entityManager.AddComponentData(e,new PhysicsDamping{Linear=0f,Angular=50f});Debug.Log($\"Física añadida a '{n}' (fricción alta, damping angular)\");}}</t>
+  </si>
+  <si>
+    <t>3.EColiComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct EColiComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;}}</t>
+  </si>
+  <si>
+    <t>4.SCerevisiaeComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct SCerevisiaeComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;public float3 GrowthDirection;}}</t>
+  </si>
+  <si>
+    <t>5.EColiSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*12345);int s=rng.NextFloat()&lt;0.5f?1:-1;Entity c=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;EColiComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.HasGeneratedChild=false;cd.Parent=entity;cd.IsInitialCell=false;cd.SeparationSign=s;float3 u=math.mul(transform.Rotation,new float3(0,s,0));ct.Position=transform.Position+u*(transform.Scale*0.25f);ecb.SetComponent(entityInQueryIndex,c,ct);ecb.SetComponent(entityInQueryIndex,c,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float off=math.lerp(0f,pd.Scale*4.9f,transform.Scale/maxScale);float3 u=math.mul(pd.Rotation,new float3(0,organism.SeparationSign,0));transform.Position=pd.Position+u*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
+  </si>
+  <si>
+    <t>6.SCerevisiaeSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*99999);float angle=rng.NextFloat(0f,math.PI*2f);float3 rnd=new float3(math.cos(angle),math.sin(angle),0f);Entity child=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;SCerevisiaeComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.IsInitialCell=false;cd.Parent=entity;cd.GrowthDirection=rnd;ct.Position=transform.Position;ecb.SetComponent(entityInQueryIndex,child,ct);ecb.SetComponent(entityInQueryIndex,child,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float r=math.clamp(transform.Scale/(organism.SeparationThreshold*maxScale),0f,1f);float off=(pd.Scale*0.5f)*r;float3 wd=math.mul(pd.Rotation,organism.GrowthDirection);transform.Position=pd.Position+wd*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Eres un modelo especializado en generar código C# para simulaciones de Unity. Considera que los tiempos son en segundos; además, los colores en Unity se expresan en valores RGB divididos en 255. Debes contestar tal cual como se te fue entrenado, sin agregar nada más de lo que se espera en C#. No puedes responder en ningún otro lenguaje de programación ni añadir comentarios o palabras innecesarias. Solo puedes responder a consultas relacionadas con simulaciones en Unity sobre e.coli, s.cerevisiae o ambas, donde se indiquen: - El color de la(s) célula(s). - El tiempo de duplicación en minutos. - El porcentaje de crecimiento para separarse del padre. Tu respuesta debe incluir estrictamente estos scripts en el orden especificado: - Si se piden ambas (e.coli y s.cerevisiae): 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.EColiComponent.cs, 4.SCerevisiaeComponent.cs, 5.EColiSystem.cs, 6.SCerevisiaeSystem.cs. - Si se pide solo e.coli: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.EColiComponent.cs, 4.EColiSystem.cs. - Si se pide solo s.cerevisiae: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.SCerevisiaeComponent.cs, 4.SCerevisiaeSystem.cs. El formato de cada script debe ser \"1.PrefabMaterialCreator.cs{...}2.CreatePrefabsOnClick.cs{...}\" etc. Cualquier pregunta que no cumpla con las características anteriores será respondida con: \"ERROR FORMATO DE PREGUNTA.\" Y recuerda, responde tal cual como se te entrenó.</t>
+  </si>
+  <si>
+    <t>1.PrefabMaterialCreator.cs{public static class PrefabMaterialCreator{const string pF=\"Assets/Resources/Prefabs\",mF=\"Assets/Resources/PrefabsMaterials\";[MenuItem(\"Tools/Crear Prefabs y Materiales\")]public static void CreatePrefabsAndMaterials(){if(!AssetDatabase.IsValidFolder(pF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"Prefabs\");Debug.Log(\"Carpeta creada: \"+pF);}if(!AssetDatabase.IsValidFolder(mF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"PrefabsMaterials\");Debug.Log(\"Carpeta creada: \"+mF);}CPAM(\"SCerevisiae\",PrimitiveType.Sphere,new Vector3(5,5,5),new Vector3(90,0,0),0);CPAM(\"EColi\",PrimitiveType.Capsule,new Vector3(.5f,2,0.5f),new Vector3(90,0,0),1);AssetDatabase.SaveAssets();AssetDatabase.Refresh();Debug.Log(\"Prefabs y materiales creados.\");}static void CPAM(string n,PrimitiveType t,Vector3 s,Vector3 r,int c){var o=GameObject.CreatePrimitive(t);o.name=n;o.transform.rotation=Quaternion.Euler(r);o.transform.localScale=s;var col=o.GetComponent&lt;Collider&gt;();if(col!=null)Object.DestroyImmediate(col);if(c==0)o.AddComponent&lt;SphereCollider&gt;();else o.AddComponent&lt;CapsuleCollider&gt;();var sh=Shader.Find(\"Universal Render Pipeline/Lit\");if(sh==null){Debug.LogError(\"Shader URP/Lit no encontrado.\");return;}var m=new Material(sh);m.color=n==\"SCerevisiae\"?new Color(0,0,1,1):n==\"EColi\"?new Color(0,1,0,1):Color.white;AssetDatabase.CreateAsset(m,Path.Combine(mF,n+\".mat\"));AssetDatabase.SaveAssets();AssetDatabase.Refresh();o.GetComponent&lt;Renderer&gt;().sharedMaterial=m;PrefabUtility.SaveAsPrefabAsset(o,Path.Combine(pF,n+\".prefab\"));Object.DestroyImmediate(o);}}}2.CreatePrefabsOnClick.cs{private void CrearEntidad(Vector3 p){if(currentPrefabIndex&gt;=prefabs.Count)return;var sQ=spawnerQuery.ToEntityArray(Allocator.Temp);if(currentPrefabIndex&gt;=sQ.Length){Debug.LogError($\"No se encontró spawner en índice {currentPrefabIndex}\");sQ.Dispose();return;}Entity s=sQ[currentPrefabIndex];sQ.Dispose();Entity pe=entityManager.GetComponentData&lt;PrefabEntityComponent&gt;(s).prefab;Entity e=entityManager.Instantiate(pe);float os=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Scale;quaternion or=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Rotation;float ry=UnityEngine.Random.Range(0f,360f);quaternion nr=math.mul(or,quaternion.RotateY(math.radians(ry)));float h=os*.5f;float3 ap=new float3(p.x,math.max(p.y+h,h),p.z);entityManager.SetComponentData(e,new LocalTransform{Position=ap,Rotation=nr,Scale=os});string n=prefabs[currentPrefabIndex].name;switch(n){case\"EColi\":entityManager.AddComponentData(e,new EColiComponent{TimeReference=1200f,SeparationThreshold=0.7f,MaxScale=1f,GrowthTime=0f,GrowthDuration=1200f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=1200f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;case\"SCerevisiae\":entityManager.AddComponentData(e,new SCerevisiaeComponent{TimeReference=5400f,SeparationThreshold=0.7f,MaxScale=5f,GrowthTime=0f,GrowthDuration=5400f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=5400f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;default:Debug.LogWarning($\"No hay componente ECS para '{n}'\");break;}AddPhysicsComponents(e,n,os);Debug.Log($\"Entidad '{n}' creada en {ap}\");}private void AddPhysicsComponents(Entity e,string n,float s){BlobAssetReference&lt;Unity.Physics.Collider&gt;c=default;Material m=new Material{Friction=8f,Restitution=0f};switch(n){case\"EColi\":c=Unity.Physics.CapsuleCollider.Create(new CapsuleGeometry{Vertex0=new float3(0,-s,0),Vertex1=new float3(0,s,0),Radius=0.25f},CollisionFilter.Default,m);break;case\"SCerevisiae\":c=Unity.Physics.SphereCollider.Create(new SphereGeometry{Center=float3.zero,Radius=s*0.1f},CollisionFilter.Default,m);break;default:Debug.LogWarning($\"No collider para '{n}'\");return;}entityManager.AddComponentData(e,new PhysicsCollider{Value=c});if(c.IsCreated){var mp=c.Value.MassProperties;entityManager.AddComponentData(e,PhysicsMass.CreateDynamic(mp,1f));}entityManager.AddComponentData(e,new PhysicsVelocity{Linear=float3.zero,Angular=float3.zero});entityManager.AddComponentData(e,new PhysicsGravityFactor{Value=1f});entityManager.AddComponentData(e,new PhysicsDamping{Linear=0f,Angular=50f});Debug.Log($\"Física añadida a '{n}' (fricción alta, damping angular)\");}}3.EColiComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct EColiComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;}}4.SCerevisiaeComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct SCerevisiaeComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;public float3 GrowthDirection;}}5.EColiSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*12345);int s=rng.NextFloat()&lt;0.5f?1:-1;Entity c=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;EColiComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.HasGeneratedChild=false;cd.Parent=entity;cd.IsInitialCell=false;cd.SeparationSign=s;float3 u=math.mul(transform.Rotation,new float3(0,s,0));ct.Position=transform.Position+u*(transform.Scale*0.25f);ecb.SetComponent(entityInQueryIndex,c,ct);ecb.SetComponent(entityInQueryIndex,c,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float off=math.lerp(0f,pd.Scale*4.9f,transform.Scale/maxScale);float3 u=math.mul(pd.Rotation,new float3(0,organism.SeparationSign,0));transform.Position=pd.Position+u*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}6.SCerevisiaeSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*99999);float angle=rng.NextFloat(0f,math.PI*2f);float3 rnd=new float3(math.cos(angle),math.sin(angle),0f);Entity child=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;SCerevisiaeComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.IsInitialCell=false;cd.Parent=entity;cd.GrowthDirection=rnd;ct.Position=transform.Position;ecb.SetComponent(entityInQueryIndex,child,ct);ecb.SetComponent(entityInQueryIndex,child,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float r=math.clamp(transform.Scale/(organism.SeparationThreshold*maxScale),0f,1f);float off=(pd.Scale*0.5f)*r;float3 wd=math.mul(pd.Rotation,organism.GrowthDirection);transform.Position=pd.Position+wd*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
   </si>
 </sst>
 </file>
@@ -177,7 +210,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0;[Red]&quot;$&quot;\-#,##0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0000;[Red]&quot;$&quot;\-#,##0.0000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +225,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -201,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,12 +248,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -232,11 +286,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6976085A-B9FC-4CD1-931F-2113AEA9B965}">
   <dimension ref="B3:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -960,17 +1024,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:K4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -979,152 +1043,297 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CA53A1-47B7-429F-9C43-38596D6DD712}">
-  <dimension ref="D5:G18"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="11" style="7"/>
+    <col min="4" max="4" width="14.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="7"/>
+    <col min="7" max="7" width="14.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" style="7"/>
+    <col min="10" max="10" width="18.5" style="7" customWidth="1"/>
+    <col min="11" max="11" width="14.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:7">
-      <c r="D5" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="D2" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="4:7">
-      <c r="D6" s="7" t="s">
+      <c r="H2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
+      <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="C3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="4:7">
-      <c r="D7">
+      <c r="D3" s="10"/>
+      <c r="H3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="8">
         <v>439</v>
       </c>
-      <c r="E7">
+      <c r="B4" s="8">
         <v>79</v>
       </c>
-      <c r="F7">
+      <c r="C4" s="8">
+        <f>B14</f>
         <v>2630</v>
       </c>
-      <c r="G7">
-        <f>SUM(D7:F7)</f>
+      <c r="D4" s="8">
+        <f>SUM(A4:C4)</f>
         <v>3148</v>
       </c>
-    </row>
-    <row r="10" spans="4:7">
-      <c r="D10" t="s">
+      <c r="H4" s="8">
+        <v>387</v>
+      </c>
+      <c r="I4" s="8">
+        <v>79</v>
+      </c>
+      <c r="J4" s="8">
+        <f>I14</f>
+        <v>2047</v>
+      </c>
+      <c r="K4" s="8">
+        <f>SUM(H4:J4)</f>
+        <v>2513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="4:7">
-      <c r="D11" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="B7" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="4:7">
-      <c r="D12" t="s">
+      <c r="C7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E12">
+      <c r="B8" s="8">
         <v>616</v>
       </c>
-      <c r="F12" s="9">
-        <f>E12/$E$18</f>
+      <c r="C8" s="9">
+        <f>B8/$B$14</f>
         <v>0.23422053231939163</v>
       </c>
-    </row>
-    <row r="13" spans="4:7">
-      <c r="D13" t="s">
+      <c r="H8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="8">
+        <v>461</v>
+      </c>
+      <c r="J8" s="9">
+        <f>I8/$I$14</f>
+        <v>0.22520762090864679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E13">
+      <c r="B9" s="8">
         <v>843</v>
       </c>
-      <c r="F13" s="9">
-        <f>E13/$E$18</f>
+      <c r="C9" s="9">
+        <f>B9/$B$14</f>
         <v>0.32053231939163496</v>
       </c>
-    </row>
-    <row r="14" spans="4:7">
-      <c r="D14" t="s">
+      <c r="H9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="8">
+        <v>757</v>
+      </c>
+      <c r="J9" s="9">
+        <f>I9/$I$14</f>
+        <v>0.36980947728383001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14">
+      <c r="B10" s="8">
         <v>87</v>
       </c>
-      <c r="F14" s="9">
-        <f t="shared" ref="F13:F17" si="0">E14/$E$18</f>
+      <c r="C10" s="9">
+        <f>B10/$B$14</f>
         <v>3.3079847908745248E-2</v>
       </c>
-    </row>
-    <row r="15" spans="4:7">
-      <c r="D15" t="s">
+      <c r="H10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="8">
+        <v>74</v>
+      </c>
+      <c r="J10" s="9">
+        <f>I10/$I$14</f>
+        <v>3.6150464093795798E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E15">
+      <c r="B11" s="8">
         <v>95</v>
       </c>
-      <c r="F15" s="9">
-        <f t="shared" si="0"/>
+      <c r="C11" s="9">
+        <f>B11/$B$14</f>
         <v>3.6121673003802278E-2</v>
       </c>
-    </row>
-    <row r="16" spans="4:7">
-      <c r="D16" t="s">
+      <c r="H11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="8">
+        <v>82</v>
+      </c>
+      <c r="J11" s="9">
+        <f>I11/$I$14</f>
+        <v>4.0058622374206154E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E16">
+      <c r="B12" s="8">
         <v>498</v>
       </c>
-      <c r="F16" s="9">
-        <f t="shared" si="0"/>
+      <c r="C12" s="9">
+        <f>B12/$B$14</f>
         <v>0.18935361216730037</v>
       </c>
-    </row>
-    <row r="17" spans="4:6">
-      <c r="D17" t="s">
+      <c r="H12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="8">
+        <v>339</v>
+      </c>
+      <c r="J12" s="9">
+        <f>I12/$I$14</f>
+        <v>0.16560820713238886</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E17">
+      <c r="B13" s="8">
         <v>491</v>
       </c>
-      <c r="F17" s="9">
-        <f t="shared" si="0"/>
+      <c r="C13" s="9">
+        <f>B13/$B$14</f>
         <v>0.18669201520912548</v>
       </c>
-    </row>
-    <row r="18" spans="4:6">
-      <c r="E18">
-        <f>SUM(E12:E17)</f>
+      <c r="H13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="8">
+        <v>334</v>
+      </c>
+      <c r="J13" s="9">
+        <f>I13/$I$14</f>
+        <v>0.16316560820713238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="8">
+        <f>SUM(B8:B13)</f>
         <v>2630</v>
       </c>
+      <c r="C14" s="9">
+        <f>B14/$B$14</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="8">
+        <f>SUM(I8:I13)</f>
+        <v>2047</v>
+      </c>
+      <c r="J14" s="9">
+        <f>I14/$I$14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" ht="15">
+      <c r="D20" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G5:G6"/>
+  <mergeCells count="2">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FIX SYSTEM CONTENT IN FINE-TUNING_v2.jsonl
</commit_message>
<xml_diff>
--- a/SimulationManager/Training LLM/TrainingStats.xlsx
+++ b/SimulationManager/Training LLM/TrainingStats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\UnityProjects\SimulationManager\Training LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3233A-12AB-40B8-BF81-2E2364588756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FAE153-8875-449E-ACAB-F0E511A51246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{21FFF4A9-BEE3-4716-82C1-DB13693BAF4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21FFF4A9-BEE3-4716-82C1-DB13693BAF4B}"/>
   </bookViews>
   <sheets>
     <sheet name="FINE-TUNING" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>MODELO</t>
   </si>
@@ -171,34 +171,37 @@
     <t>NUEVO DESGLOSE RESPUESTA ASSISTANT</t>
   </si>
   <si>
-    <t>1.PrefabMaterialCreator.cs{public static class PrefabMaterialCreator{const string pF=\"Assets/Resources/Prefabs\",mF=\"Assets/Resources/PrefabsMaterials\";[MenuItem(\"Tools/Crear Prefabs y Materiales\")]public static void CreatePrefabsAndMaterials(){if(!AssetDatabase.IsValidFolder(pF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"Prefabs\");Debug.Log(\"Carpeta creada: \"+pF);}if(!AssetDatabase.IsValidFolder(mF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"PrefabsMaterials\");Debug.Log(\"Carpeta creada: \"+mF);}CPAM(\"SCerevisiae\",PrimitiveType.Sphere,new Vector3(5,5,5),new Vector3(90,0,0),0);CPAM(\"EColi\",PrimitiveType.Capsule,new Vector3(.5f,2,0.5f),new Vector3(90,0,0),1);AssetDatabase.SaveAssets();AssetDatabase.Refresh();Debug.Log(\"Prefabs y materiales creados.\");}static void CPAM(string n,PrimitiveType t,Vector3 s,Vector3 r,int c){var o=GameObject.CreatePrimitive(t);o.name=n;o.transform.rotation=Quaternion.Euler(r);o.transform.localScale=s;var col=o.GetComponent&lt;Collider&gt;();if(col!=null)Object.DestroyImmediate(col);if(c==0)o.AddComponent&lt;SphereCollider&gt;();else o.AddComponent&lt;CapsuleCollider&gt;();var sh=Shader.Find(\"Universal Render Pipeline/Lit\");if(sh==null){Debug.LogError(\"Shader URP/Lit no encontrado.\");return;}var m=new Material(sh);m.color=n==\"SCerevisiae\"?new Color(0,0,1,1):n==\"EColi\"?new Color(0,1,0,1):Color.white;AssetDatabase.CreateAsset(m,Path.Combine(mF,n+\".mat\"));AssetDatabase.SaveAssets();AssetDatabase.Refresh();o.GetComponent&lt;Renderer&gt;().sharedMaterial=m;PrefabUtility.SaveAsPrefabAsset(o,Path.Combine(pF,n+\".prefab\"));Object.DestroyImmediate(o);}}}</t>
-  </si>
-  <si>
-    <t>2.CreatePrefabsOnClick.cs{private void CrearEntidad(Vector3 p){if(currentPrefabIndex&gt;=prefabs.Count)return;var sQ=spawnerQuery.ToEntityArray(Allocator.Temp);if(currentPrefabIndex&gt;=sQ.Length){Debug.LogError($\"No se encontró spawner en índice {currentPrefabIndex}\");sQ.Dispose();return;}Entity s=sQ[currentPrefabIndex];sQ.Dispose();Entity pe=entityManager.GetComponentData&lt;PrefabEntityComponent&gt;(s).prefab;Entity e=entityManager.Instantiate(pe);float os=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Scale;quaternion or=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Rotation;float ry=UnityEngine.Random.Range(0f,360f);quaternion nr=math.mul(or,quaternion.RotateY(math.radians(ry)));float h=os*.5f;float3 ap=new float3(p.x,math.max(p.y+h,h),p.z);entityManager.SetComponentData(e,new LocalTransform{Position=ap,Rotation=nr,Scale=os});string n=prefabs[currentPrefabIndex].name;switch(n){case\"EColi\":entityManager.AddComponentData(e,new EColiComponent{TimeReference=1200f,SeparationThreshold=0.7f,MaxScale=1f,GrowthTime=0f,GrowthDuration=1200f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=1200f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;case\"SCerevisiae\":entityManager.AddComponentData(e,new SCerevisiaeComponent{TimeReference=5400f,SeparationThreshold=0.7f,MaxScale=5f,GrowthTime=0f,GrowthDuration=5400f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=5400f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;default:Debug.LogWarning($\"No hay componente ECS para '{n}'\");break;}AddPhysicsComponents(e,n,os);Debug.Log($\"Entidad '{n}' creada en {ap}\");}private void AddPhysicsComponents(Entity e,string n,float s){BlobAssetReference&lt;Unity.Physics.Collider&gt;c=default;Material m=new Material{Friction=8f,Restitution=0f};switch(n){case\"EColi\":c=Unity.Physics.CapsuleCollider.Create(new CapsuleGeometry{Vertex0=new float3(0,-s,0),Vertex1=new float3(0,s,0),Radius=0.25f},CollisionFilter.Default,m);break;case\"SCerevisiae\":c=Unity.Physics.SphereCollider.Create(new SphereGeometry{Center=float3.zero,Radius=s*0.1f},CollisionFilter.Default,m);break;default:Debug.LogWarning($\"No collider para '{n}'\");return;}entityManager.AddComponentData(e,new PhysicsCollider{Value=c});if(c.IsCreated){var mp=c.Value.MassProperties;entityManager.AddComponentData(e,PhysicsMass.CreateDynamic(mp,1f));}entityManager.AddComponentData(e,new PhysicsVelocity{Linear=float3.zero,Angular=float3.zero});entityManager.AddComponentData(e,new PhysicsGravityFactor{Value=1f});entityManager.AddComponentData(e,new PhysicsDamping{Linear=0f,Angular=50f});Debug.Log($\"Física añadida a '{n}' (fricción alta, damping angular)\");}}</t>
-  </si>
-  <si>
-    <t>3.EColiComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct EColiComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;}}</t>
-  </si>
-  <si>
-    <t>4.SCerevisiaeComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct SCerevisiaeComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;public float3 GrowthDirection;}}</t>
-  </si>
-  <si>
-    <t>5.EColiSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*12345);int s=rng.NextFloat()&lt;0.5f?1:-1;Entity c=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;EColiComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.HasGeneratedChild=false;cd.Parent=entity;cd.IsInitialCell=false;cd.SeparationSign=s;float3 u=math.mul(transform.Rotation,new float3(0,s,0));ct.Position=transform.Position+u*(transform.Scale*0.25f);ecb.SetComponent(entityInQueryIndex,c,ct);ecb.SetComponent(entityInQueryIndex,c,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float off=math.lerp(0f,pd.Scale*4.9f,transform.Scale/maxScale);float3 u=math.mul(pd.Rotation,new float3(0,organism.SeparationSign,0));transform.Position=pd.Position+u*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
-  </si>
-  <si>
-    <t>6.SCerevisiaeSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*99999);float angle=rng.NextFloat(0f,math.PI*2f);float3 rnd=new float3(math.cos(angle),math.sin(angle),0f);Entity child=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;SCerevisiaeComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.IsInitialCell=false;cd.Parent=entity;cd.GrowthDirection=rnd;ct.Position=transform.Position;ecb.SetComponent(entityInQueryIndex,child,ct);ecb.SetComponent(entityInQueryIndex,child,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float r=math.clamp(transform.Scale/(organism.SeparationThreshold*maxScale),0f,1f);float off=(pd.Scale*0.5f)*r;float3 wd=math.mul(pd.Rotation,organism.GrowthDirection);transform.Position=pd.Position+wd*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>Eres un modelo especializado en generar código C# para simulaciones de Unity. Considera que los tiempos son en segundos; además, los colores en Unity se expresan en valores RGB divididos en 255. Debes contestar tal cual como se te fue entrenado, sin agregar nada más de lo que se espera en C#. No puedes responder en ningún otro lenguaje de programación ni añadir comentarios o palabras innecesarias. Solo puedes responder a consultas relacionadas con simulaciones en Unity sobre e.coli, s.cerevisiae o ambas, donde se indiquen: - El color de la(s) célula(s). - El tiempo de duplicación en minutos. - El porcentaje de crecimiento para separarse del padre. Tu respuesta debe incluir estrictamente estos scripts en el orden especificado: - Si se piden ambas (e.coli y s.cerevisiae): 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.EColiComponent.cs, 4.SCerevisiaeComponent.cs, 5.EColiSystem.cs, 6.SCerevisiaeSystem.cs. - Si se pide solo e.coli: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.EColiComponent.cs, 4.EColiSystem.cs. - Si se pide solo s.cerevisiae: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.SCerevisiaeComponent.cs, 4.SCerevisiaeSystem.cs. El formato de cada script debe ser \"1.PrefabMaterialCreator.cs{...}2.CreatePrefabsOnClick.cs{...}\" etc. Cualquier pregunta que no cumpla con las características anteriores será respondida con: \"ERROR FORMATO DE PREGUNTA.\" Y recuerda, responde tal cual como se te entrenó.</t>
-  </si>
-  <si>
-    <t>1.PrefabMaterialCreator.cs{public static class PrefabMaterialCreator{const string pF=\"Assets/Resources/Prefabs\",mF=\"Assets/Resources/PrefabsMaterials\";[MenuItem(\"Tools/Crear Prefabs y Materiales\")]public static void CreatePrefabsAndMaterials(){if(!AssetDatabase.IsValidFolder(pF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"Prefabs\");Debug.Log(\"Carpeta creada: \"+pF);}if(!AssetDatabase.IsValidFolder(mF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"PrefabsMaterials\");Debug.Log(\"Carpeta creada: \"+mF);}CPAM(\"SCerevisiae\",PrimitiveType.Sphere,new Vector3(5,5,5),new Vector3(90,0,0),0);CPAM(\"EColi\",PrimitiveType.Capsule,new Vector3(.5f,2,0.5f),new Vector3(90,0,0),1);AssetDatabase.SaveAssets();AssetDatabase.Refresh();Debug.Log(\"Prefabs y materiales creados.\");}static void CPAM(string n,PrimitiveType t,Vector3 s,Vector3 r,int c){var o=GameObject.CreatePrimitive(t);o.name=n;o.transform.rotation=Quaternion.Euler(r);o.transform.localScale=s;var col=o.GetComponent&lt;Collider&gt;();if(col!=null)Object.DestroyImmediate(col);if(c==0)o.AddComponent&lt;SphereCollider&gt;();else o.AddComponent&lt;CapsuleCollider&gt;();var sh=Shader.Find(\"Universal Render Pipeline/Lit\");if(sh==null){Debug.LogError(\"Shader URP/Lit no encontrado.\");return;}var m=new Material(sh);m.color=n==\"SCerevisiae\"?new Color(0,0,1,1):n==\"EColi\"?new Color(0,1,0,1):Color.white;AssetDatabase.CreateAsset(m,Path.Combine(mF,n+\".mat\"));AssetDatabase.SaveAssets();AssetDatabase.Refresh();o.GetComponent&lt;Renderer&gt;().sharedMaterial=m;PrefabUtility.SaveAsPrefabAsset(o,Path.Combine(pF,n+\".prefab\"));Object.DestroyImmediate(o);}}}2.CreatePrefabsOnClick.cs{private void CrearEntidad(Vector3 p){if(currentPrefabIndex&gt;=prefabs.Count)return;var sQ=spawnerQuery.ToEntityArray(Allocator.Temp);if(currentPrefabIndex&gt;=sQ.Length){Debug.LogError($\"No se encontró spawner en índice {currentPrefabIndex}\");sQ.Dispose();return;}Entity s=sQ[currentPrefabIndex];sQ.Dispose();Entity pe=entityManager.GetComponentData&lt;PrefabEntityComponent&gt;(s).prefab;Entity e=entityManager.Instantiate(pe);float os=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Scale;quaternion or=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Rotation;float ry=UnityEngine.Random.Range(0f,360f);quaternion nr=math.mul(or,quaternion.RotateY(math.radians(ry)));float h=os*.5f;float3 ap=new float3(p.x,math.max(p.y+h,h),p.z);entityManager.SetComponentData(e,new LocalTransform{Position=ap,Rotation=nr,Scale=os});string n=prefabs[currentPrefabIndex].name;switch(n){case\"EColi\":entityManager.AddComponentData(e,new EColiComponent{TimeReference=1200f,SeparationThreshold=0.7f,MaxScale=1f,GrowthTime=0f,GrowthDuration=1200f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=1200f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;case\"SCerevisiae\":entityManager.AddComponentData(e,new SCerevisiaeComponent{TimeReference=5400f,SeparationThreshold=0.7f,MaxScale=5f,GrowthTime=0f,GrowthDuration=5400f*0.7f,TimeSinceLastDivision=0f,DivisionInterval=5400f*0.7f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;default:Debug.LogWarning($\"No hay componente ECS para '{n}'\");break;}AddPhysicsComponents(e,n,os);Debug.Log($\"Entidad '{n}' creada en {ap}\");}private void AddPhysicsComponents(Entity e,string n,float s){BlobAssetReference&lt;Unity.Physics.Collider&gt;c=default;Material m=new Material{Friction=8f,Restitution=0f};switch(n){case\"EColi\":c=Unity.Physics.CapsuleCollider.Create(new CapsuleGeometry{Vertex0=new float3(0,-s,0),Vertex1=new float3(0,s,0),Radius=0.25f},CollisionFilter.Default,m);break;case\"SCerevisiae\":c=Unity.Physics.SphereCollider.Create(new SphereGeometry{Center=float3.zero,Radius=s*0.1f},CollisionFilter.Default,m);break;default:Debug.LogWarning($\"No collider para '{n}'\");return;}entityManager.AddComponentData(e,new PhysicsCollider{Value=c});if(c.IsCreated){var mp=c.Value.MassProperties;entityManager.AddComponentData(e,PhysicsMass.CreateDynamic(mp,1f));}entityManager.AddComponentData(e,new PhysicsVelocity{Linear=float3.zero,Angular=float3.zero});entityManager.AddComponentData(e,new PhysicsGravityFactor{Value=1f});entityManager.AddComponentData(e,new PhysicsDamping{Linear=0f,Angular=50f});Debug.Log($\"Física añadida a '{n}' (fricción alta, damping angular)\");}}3.EColiComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct EColiComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;}}4.SCerevisiaeComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct SCerevisiaeComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell;public Entity Parent;public int SeparationSign;public float3 GrowthDirection;}}5.EColiSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*12345);int s=rng.NextFloat()&lt;0.5f?1:-1;Entity c=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;EColiComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.HasGeneratedChild=false;cd.Parent=entity;cd.IsInitialCell=false;cd.SeparationSign=s;float3 u=math.mul(transform.Rotation,new float3(0,s,0));ct.Position=transform.Position+u*(transform.Scale*0.25f);ecb.SetComponent(entityInQueryIndex,c,ct);ecb.SetComponent(entityInQueryIndex,c,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float off=math.lerp(0f,pd.Scale*4.9f,transform.Scale/maxScale);float3 u=math.mul(pd.Rotation,new float3(0,organism.SeparationSign,0));transform.Position=pd.Position+u*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}6.SCerevisiaeSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*99999);float angle=rng.NextFloat(0f,math.PI*2f);float3 rnd=new float3(math.cos(angle),math.sin(angle),0f);Entity child=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;SCerevisiaeComponent cd=organism;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.IsInitialCell=false;cd.Parent=entity;cd.GrowthDirection=rnd;ct.Position=transform.Position;ecb.SetComponent(entityInQueryIndex,child,ct);ecb.SetComponent(entityInQueryIndex,child,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float r=math.clamp(transform.Scale/(organism.SeparationThreshold*maxScale),0f,1f);float off=(pd.Scale*0.5f)*r;float3 wd=math.mul(pd.Rotation,organism.GrowthDirection);transform.Position=pd.Position+wd*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
+    <t>Eres un modelo especializado en generar código C# para simulaciones de Unity. Considera que los tiempos son en segundos; además, los colores en Unity se expresan en valores RGB divididos en 255. Debes contestar tal cual como se te fue entrenado, sin agregar nada más de lo que se espera en C#. No puedes responder en ningún otro lenguaje de programación ni añadir comentarios o palabras innecesarias. Solo puedes responder a consultas relacionadas con simulaciones en Unity sobre EColi, SCerevisiae o ambas, donde se indiquen: - El color de la(s) célula(s). - El tiempo de duplicación en minutos. - El porcentaje de crecimiento para separarse del padre. Tu respuesta debe incluir estrictamente estos scripts en el orden especificado: - Si se piden ambas (EColi y SCerevisiae): 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.EColiComponent.cs, 4.SCerevisiaeComponent.cs, 5.EColiSystem.cs, 6.SCerevisiaeSystem.cs. - Si se pide solo EColi: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.EColiComponent.cs, 4.EColiSystem.cs. - Si se pide solo SCerevisiae: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.SCerevisiaeComponent.cs, 4.SCerevisiaeSystem.cs - Si se pide 2 EColi: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.EColi_1Component.cs, 4.EColi_2Component.cs, 5.EColi_1System.cs, 6.EColi_2System.cs. - Si se pide 2 SCerevisiae: 1.PrefabMaterialCreator.cs, 2.CreatePrefabsOnClick.cs, 3.SCerevisiae_1Component.cs, 4.SCerevisiae_2Component.cs, 5.SCerevisiae_1System.cs, 6.SCerevisiae_2System.cs. El formato de cada script debe ser \"1.PrefabMaterialCreator.cs{...}2.CreatePrefabsOnClick.cs{...}\" etc. Cualquier pregunta que no cumpla con las características anteriores será respondida con: \"ERROR FORMATO DE PREGUNTA.\".</t>
+  </si>
+  <si>
+    <t>1.PrefabMaterialCreator.cs{public static class PrefabMaterialCreator{const string pF=\"Assets/Resources/Prefabs\",mF=\"Assets/Resources/PrefabsMaterials\";[MenuItem(\"Tools/Crear Prefabs y Materiales\")]public static void CreatePrefabsAndMaterials(){if(!AssetDatabase.IsValidFolder(pF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"Prefabs\");Debug.Log(\"Carpeta creada: \"+pF);}if(!AssetDatabase.IsValidFolder(mF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"PrefabsMaterials\");Debug.Log(\"Carpeta creada: \"+mF);}CPAM(\"SCerevisiae\",PrimitiveType.Sphere,new Vector3(5,5,5),new Vector3(90,0,0),0);CPAM(\"EColi\",PrimitiveType.Capsule,new Vector3(.5f,2,0.5f),new Vector3(90,0,0),1);AssetDatabase.SaveAssets();AssetDatabase.Refresh();Debug.Log(\"Prefabs y materiales creados.\");}static void CPAM(string n,PrimitiveType t,Vector3 s,Vector3 r,int c){var o=GameObject.CreatePrimitive(t);o.name=n;o.transform.rotation=Quaternion.Euler(r);o.transform.localScale=s;var col=o.GetComponent&lt;Collider&gt;();if(col!=null)Object.DestroyImmediate(col);if(c==0)o.AddComponent&lt;SphereCollider&gt;();else o.AddComponent&lt;CapsuleCollider&gt;();var sh=Shader.Find(\"Universal Render Pipeline/Lit\");if(sh==null){Debug.LogError(\"Shader URP/Lit no encontrado.\");return;}var m=new Material(sh);m.color=n==\"SCerevisiae\"?new Color(0.25f,0.88f,0.82f,1):n==\"EColi\"?new Color(0.5f,0,0.5f,1):Color.white;AssetDatabase.CreateAsset(m,Path.Combine(mF,n+\".mat\"));AssetDatabase.SaveAssets();AssetDatabase.Refresh();o.GetComponent&lt;Renderer&gt;().sharedMaterial=m;PrefabUtility.SaveAsPrefabAsset(o,Path.Combine(pF,n+\".prefab\"));Object.DestroyImmediate(o);}}}2.CreatePrefabsOnClick.cs{private void CrearEntidad(Vector3 p){if(currentPrefabIndex&gt;=prefabs.Count)return;var sQ=spawnerQuery.ToEntityArray(Allocator.Temp);if(currentPrefabIndex&gt;=sQ.Length){Debug.LogError($\"No se encontró spawner en índice {currentPrefabIndex}\");sQ.Dispose();return;}Entity s=sQ[currentPrefabIndex];sQ.Dispose();Entity pe=entityManager.GetComponentData&lt;PrefabEntityComponent&gt;(s).prefab;Entity e=entityManager.Instantiate(pe);float os=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Scale;quaternion or=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Rotation;float ry=UnityEngine.Random.Range(0f,360f);quaternion nr=math.mul(or,quaternion.RotateY(math.radians(ry)));float h=os*.5f;float3 ap=new float3(p.x,math.max(p.y+h,h),p.z);entityManager.SetComponentData(e,new LocalTransform{Position=ap,Rotation=nr,Scale=os});string n=prefabs[currentPrefabIndex].name;switch(n){case \"EColi\":entityManager.AddComponentData(e,new EColiComponent{TimeReference=1080f,SeparationThreshold=0.65f,MaxScale=1f,GrowthTime=0f,GrowthDuration=1080f*0.65f,TimeSinceLastDivision=0f,DivisionInterval=1080f*0.65f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;case \"SCerevisiae\":entityManager.AddComponentData(e,new SCerevisiaeComponent{TimeReference=2700f,SeparationThreshold=0.75f,MaxScale=5f,GrowthTime=0f,GrowthDuration=2700f*0.75f,TimeSinceLastDivision=0f,DivisionInterval=2700f*0.75f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;default:Debug.LogWarning($\"No hay componente ECS para '{n}'\");break;}AddPhysicsComponents(e,n,os);Debug.Log($\"Entidad '{n}' creada en {ap}\");}private void AddPhysicsComponents(Entity e,string n,float s){BlobAssetReference&lt;Unity.Physics.Collider&gt; c=default;Material m=new Material{Friction=8f,Restitution=0f};switch(n){case \"EColi\":c=Unity.Physics.CapsuleCollider.Create(new CapsuleGeometry{Vertex0=new float3(0,-s,0),Vertex1=new float3(0,s,0),Radius=0.25f},CollisionFilter.Default,m);break;case \"SCerevisiae\":c=Unity.Physics.SphereCollider.Create(new SphereGeometry{Center=float3.zero,Radius=s*0.1f},CollisionFilter.Default,m);break;default:Debug.LogWarning($\"No collider para '{n}'\");return;}entityManager.AddComponentData(e,new PhysicsCollider{Value=c});if(c.IsCreated){var mp=c.Value.MassProperties;entityManager.AddComponentData(e,PhysicsMass.CreateDynamic(mp,1f));}entityManager.AddComponentData(e,new PhysicsVelocity{Linear=float3.zero,Angular=float3.zero});entityManager.AddComponentData(e,new PhysicsGravityFactor{Value=1f});entityManager.AddComponentData(e,new PhysicsDamping{Linear=0f,Angular=50f});Debug.Log($\"Física añadida a '{n}' (fricción alta, damping angular)\");}}3.EColiComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct EColiComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell,TimeReferenceInitialized;public Entity Parent;public int SeparationSign;}}4.SCerevisiaeComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct SCerevisiaeComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell,TimeReferenceInitialized;public Entity Parent;public int SeparationSign;public float3 GrowthDirection;}}5.EColiSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*12345);int s=rng.NextFloat()&lt;0.5f?1:-1;Entity c=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;EColiComponent cd=organism;cd.TimeReferenceInitialized = false;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.HasGeneratedChild=false;cd.Parent=entity;cd.IsInitialCell=false;cd.SeparationSign=s;float3 u=math.mul(transform.Rotation,new float3(0,s,0));ct.Position=transform.Position+u*(transform.Scale*0.25f);ecb.SetComponent(entityInQueryIndex,c,ct);ecb.SetComponent(entityInQueryIndex,c,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float off=math.lerp(0f,pd.Scale*4.9f,transform.Scale/maxScale);float3 u=math.mul(pd.Rotation,new float3(0,organism.SeparationSign,0));transform.Position=pd.Position+u*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}6.SCerevisiaeSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*99999);float angle=rng.NextFloat(0f,math.PI*2f);float3 rnd=new float3(math.cos(angle),math.sin(angle),0f);Entity child=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;SCerevisiaeComponent cd=organism;cd.TimeReferenceInitialized = false;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.IsInitialCell=false;cd.Parent=entity;cd.GrowthDirection=rnd;ct.Position=transform.Position;ecb.SetComponent(entityInQueryIndex,child,ct);ecb.SetComponent(entityInQueryIndex,child,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float r=math.clamp(transform.Scale/(organism.SeparationThreshold*maxScale),0f,1f);float off=(pd.Scale*0.5f)*r;float3 wd=math.mul(pd.Rotation,organism.GrowthDirection);transform.Position=pd.Position+wd*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
+  </si>
+  <si>
+    <t>1.PrefabMaterialCreator.cs{public static class PrefabMaterialCreator{const string pF=\"Assets/Resources/Prefabs\",mF=\"Assets/Resources/PrefabsMaterials\";[MenuItem(\"Tools/Crear Prefabs y Materiales\")]public static void CreatePrefabsAndMaterials(){if(!AssetDatabase.IsValidFolder(pF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"Prefabs\");Debug.Log(\"Carpeta creada: \"+pF);}if(!AssetDatabase.IsValidFolder(mF)){AssetDatabase.CreateFolder(\"Assets/Resources\",\"PrefabsMaterials\");Debug.Log(\"Carpeta creada: \"+mF);}CPAM(\"SCerevisiae\",PrimitiveType.Sphere,new Vector3(5,5,5),new Vector3(90,0,0),0);CPAM(\"EColi\",PrimitiveType.Capsule,new Vector3(.5f,2,0.5f),new Vector3(90,0,0),1);AssetDatabase.SaveAssets();AssetDatabase.Refresh();Debug.Log(\"Prefabs y materiales creados.\");}static void CPAM(string n,PrimitiveType t,Vector3 s,Vector3 r,int c){var o=GameObject.CreatePrimitive(t);o.name=n;o.transform.rotation=Quaternion.Euler(r);o.transform.localScale=s;var col=o.GetComponent&lt;Collider&gt;();if(col!=null)Object.DestroyImmediate(col);if(c==0)o.AddComponent&lt;SphereCollider&gt;();else o.AddComponent&lt;CapsuleCollider&gt;();var sh=Shader.Find(\"Universal Render Pipeline/Lit\");if(sh==null){Debug.LogError(\"Shader URP/Lit no encontrado.\");return;}var m=new Material(sh);m.color=n==\"SCerevisiae\"?new Color(0.25f,0.88f,0.82f,1):n==\"EColi\"?new Color(0.5f,0,0.5f,1):Color.white;AssetDatabase.CreateAsset(m,Path.Combine(mF,n+\".mat\"));AssetDatabase.SaveAssets();AssetDatabase.Refresh();o.GetComponent&lt;Renderer&gt;().sharedMaterial=m;PrefabUtility.SaveAsPrefabAsset(o,Path.Combine(pF,n+\".prefab\"));Object.DestroyImmediate(o);}}}</t>
+  </si>
+  <si>
+    <t>2.CreatePrefabsOnClick.cs{private void CrearEntidad(Vector3 p){if(currentPrefabIndex&gt;=prefabs.Count)return;var sQ=spawnerQuery.ToEntityArray(Allocator.Temp);if(currentPrefabIndex&gt;=sQ.Length){Debug.LogError($\"No se encontró spawner en índice {currentPrefabIndex}\");sQ.Dispose();return;}Entity s=sQ[currentPrefabIndex];sQ.Dispose();Entity pe=entityManager.GetComponentData&lt;PrefabEntityComponent&gt;(s).prefab;Entity e=entityManager.Instantiate(pe);float os=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Scale;quaternion or=entityManager.GetComponentData&lt;LocalTransform&gt;(pe).Rotation;float ry=UnityEngine.Random.Range(0f,360f);quaternion nr=math.mul(or,quaternion.RotateY(math.radians(ry)));float h=os*.5f;float3 ap=new float3(p.x,math.max(p.y+h,h),p.z);entityManager.SetComponentData(e,new LocalTransform{Position=ap,Rotation=nr,Scale=os});string n=prefabs[currentPrefabIndex].name;switch(n){case \"EColi\":entityManager.AddComponentData(e,new EColiComponent{TimeReference=1080f,SeparationThreshold=0.65f,MaxScale=1f,GrowthTime=0f,GrowthDuration=1080f*0.65f,TimeSinceLastDivision=0f,DivisionInterval=1080f*0.65f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;case \"SCerevisiae\":entityManager.AddComponentData(e,new SCerevisiaeComponent{TimeReference=2700f,SeparationThreshold=0.75f,MaxScale=5f,GrowthTime=0f,GrowthDuration=2700f*0.75f,TimeSinceLastDivision=0f,DivisionInterval=2700f*0.75f,HasGeneratedChild=false,Parent=Entity.Null,IsInitialCell=true,SeparationSign=0});break;default:Debug.LogWarning($\"No hay componente ECS para '{n}'\");break;}AddPhysicsComponents(e,n,os);Debug.Log($\"Entidad '{n}' creada en {ap}\");}private void AddPhysicsComponents(Entity e,string n,float s){BlobAssetReference&lt;Unity.Physics.Collider&gt; c=default;Material m=new Material{Friction=8f,Restitution=0f};switch(n){case \"EColi\":c=Unity.Physics.CapsuleCollider.Create(new CapsuleGeometry{Vertex0=new float3(0,-s,0),Vertex1=new float3(0,s,0),Radius=0.25f},CollisionFilter.Default,m);break;case \"SCerevisiae\":c=Unity.Physics.SphereCollider.Create(new SphereGeometry{Center=float3.zero,Radius=s*0.1f},CollisionFilter.Default,m);break;default:Debug.LogWarning($\"No collider para '{n}'\");return;}entityManager.AddComponentData(e,new PhysicsCollider{Value=c});if(c.IsCreated){var mp=c.Value.MassProperties;entityManager.AddComponentData(e,PhysicsMass.CreateDynamic(mp,1f));}entityManager.AddComponentData(e,new PhysicsVelocity{Linear=float3.zero,Angular=float3.zero});entityManager.AddComponentData(e,new PhysicsGravityFactor{Value=1f});entityManager.AddComponentData(e,new PhysicsDamping{Linear=0f,Angular=50f});Debug.Log($\"Física añadida a '{n}' (fricción alta, damping angular)\");}}</t>
+  </si>
+  <si>
+    <t>3.EColiComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct EColiComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell,TimeReferenceInitialized;public Entity Parent;public int SeparationSign;}}</t>
+  </si>
+  <si>
+    <t>4.SCerevisiaeComponent.cs{using Unity.Entities;using Unity.Mathematics;public struct SCerevisiaeComponent:IComponentData{public float TimeReference,MaxScale,GrowthTime,GrowthDuration,TimeSinceLastDivision,DivisionInterval,SeparationThreshold;public bool HasGeneratedChild,IsInitialCell,TimeReferenceInitialized;public Entity Parent;public int SeparationSign;public float3 GrowthDirection;}}</t>
+  </si>
+  <si>
+    <t>6.SCerevisiaeSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*99999);float angle=rng.NextFloat(0f,math.PI*2f);float3 rnd=new float3(math.cos(angle),math.sin(angle),0f);Entity child=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;SCerevisiaeComponent cd=organism;cd.TimeReferenceInitialized = false;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.IsInitialCell=false;cd.Parent=entity;cd.GrowthDirection=rnd;ct.Position=transform.Position;ecb.SetComponent(entityInQueryIndex,child,ct);ecb.SetComponent(entityInQueryIndex,child,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float r=math.clamp(transform.Scale/(organism.SeparationThreshold*maxScale),0f,1f);float off=(pd.Scale*0.5f)*r;float3 wd=math.mul(pd.Rotation,organism.GrowthDirection);transform.Position=pd.Position+wd*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
+  </si>
+  <si>
+    <t>5.EColiSystem.cs{if(transform.Scale&gt;=maxScale){organism.TimeSinceLastDivision+=deltaTime;if(organism.TimeSinceLastDivision&gt;=organism.DivisionInterval){Unity.Mathematics.Random rng=new Unity.Mathematics.Random((uint)(entityInQueryIndex+1)*12345);int s=rng.NextFloat()&lt;0.5f?1:-1;Entity c=ecb.Instantiate(entityInQueryIndex,entity);LocalTransform ct=transform;ct.Scale=0.01f;EColiComponent cd=organism;cd.TimeReferenceInitialized = false;cd.GrowthTime=0f;cd.TimeSinceLastDivision=0f;cd.HasGeneratedChild=false;cd.Parent=entity;cd.IsInitialCell=false;cd.SeparationSign=s;float3 u=math.mul(transform.Rotation,new float3(0,s,0));ct.Position=transform.Position+u*(transform.Scale*0.25f);ecb.SetComponent(entityInQueryIndex,c,ct);ecb.SetComponent(entityInQueryIndex,c,cd);organism.TimeSinceLastDivision=0f;}}if(!organism.IsInitialCell&amp;&amp;organism.Parent!=Entity.Null&amp;&amp;parentMap.TryGetValue(organism.Parent,out ParentData pd)){if(transform.Scale&lt;organism.SeparationThreshold*maxScale){float off=math.lerp(0f,pd.Scale*4.9f,transform.Scale/maxScale);float3 u=math.mul(pd.Rotation,new float3(0,organism.SeparationSign,0));transform.Position=pd.Position+u*off;transform.Rotation=pd.Rotation;}else organism.Parent=Entity.Null;}}</t>
+  </si>
+  <si>
+    <t>*TODO CONSIDERANDO UNA LINEA DE JSONL PROMEDIO</t>
   </si>
 </sst>
 </file>
@@ -284,9 +287,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -295,10 +295,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -638,55 +641,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6976085A-B9FC-4CD1-931F-2113AEA9B965}">
   <dimension ref="B3:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="3" spans="2:17">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
@@ -708,13 +711,13 @@
       <c r="J4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="2:17" ht="28.5" customHeight="1">
       <c r="B5" s="1">
@@ -1024,17 +1027,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:K4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1043,292 +1046,295 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CA53A1-47B7-429F-9C43-38596D6DD712}">
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="3" width="11" style="7"/>
-    <col min="4" max="4" width="14.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11" style="7"/>
-    <col min="7" max="7" width="14.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11" style="7"/>
-    <col min="10" max="10" width="18.5" style="7" customWidth="1"/>
-    <col min="11" max="11" width="14.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="7"/>
+    <col min="1" max="3" width="11" style="6"/>
+    <col min="4" max="4" width="14.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="6"/>
+    <col min="7" max="7" width="14.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" style="6"/>
+    <col min="10" max="10" width="18.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="14.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="8" t="s">
+      <c r="M2" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="H3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="D3" s="11"/>
+      <c r="H3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="8">
+      <c r="J3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="7">
         <v>439</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>79</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <f>B14</f>
         <v>2630</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>SUM(A4:C4)</f>
         <v>3148</v>
       </c>
-      <c r="H4" s="8">
-        <v>387</v>
-      </c>
-      <c r="I4" s="8">
+      <c r="H4" s="7">
+        <v>513</v>
+      </c>
+      <c r="I4" s="7">
         <v>79</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <f>I14</f>
-        <v>2047</v>
-      </c>
-      <c r="K4" s="8">
+        <v>2093</v>
+      </c>
+      <c r="K4" s="7">
         <f>SUM(H4:J4)</f>
-        <v>2513</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="8" t="s">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="H6" s="8" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="H6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="8" t="s">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="7">
+        <v>616</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" ref="C8:C14" si="0">B8/$B$14</f>
+        <v>0.23422053231939163</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="7">
+        <v>476</v>
+      </c>
+      <c r="J8" s="8">
+        <f t="shared" ref="J8:J14" si="1">I8/$I$14</f>
+        <v>0.22742474916387959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="7">
+        <v>843</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.32053231939163496</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="7">
+        <v>766</v>
+      </c>
+      <c r="J9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.36598184424271379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="7">
+        <v>87</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3079847908745248E-2</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="7">
+        <v>78</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" si="1"/>
+        <v>3.7267080745341616E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="7">
+        <v>95</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="0"/>
+        <v>3.6121673003802278E-2</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="8">
-        <v>616</v>
-      </c>
-      <c r="C8" s="9">
-        <f>B8/$B$14</f>
-        <v>0.23422053231939163</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="I11" s="7">
+        <v>86</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" si="1"/>
+        <v>4.1089345437171527E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="7">
+        <v>498</v>
+      </c>
+      <c r="C12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18935361216730037</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="7">
+        <v>346</v>
+      </c>
+      <c r="J12" s="8">
+        <f t="shared" si="1"/>
+        <v>0.16531294792164358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="7">
+        <v>491</v>
+      </c>
+      <c r="C13" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18669201520912548</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="7">
+        <v>341</v>
+      </c>
+      <c r="J13" s="8">
+        <f t="shared" si="1"/>
+        <v>0.16292403248924989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="8">
-        <v>461</v>
-      </c>
-      <c r="J8" s="9">
-        <f>I8/$I$14</f>
-        <v>0.22520762090864679</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="8">
-        <v>843</v>
-      </c>
-      <c r="C9" s="9">
-        <f>B9/$B$14</f>
-        <v>0.32053231939163496</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="8">
-        <v>757</v>
-      </c>
-      <c r="J9" s="9">
-        <f>I9/$I$14</f>
-        <v>0.36980947728383001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="8">
-        <v>87</v>
-      </c>
-      <c r="C10" s="9">
-        <f>B10/$B$14</f>
-        <v>3.3079847908745248E-2</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="8">
-        <v>74</v>
-      </c>
-      <c r="J10" s="9">
-        <f>I10/$I$14</f>
-        <v>3.6150464093795798E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="8">
-        <v>95</v>
-      </c>
-      <c r="C11" s="9">
-        <f>B11/$B$14</f>
-        <v>3.6121673003802278E-2</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="8">
-        <v>82</v>
-      </c>
-      <c r="J11" s="9">
-        <f>I11/$I$14</f>
-        <v>4.0058622374206154E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="8">
-        <v>498</v>
-      </c>
-      <c r="C12" s="9">
-        <f>B12/$B$14</f>
-        <v>0.18935361216730037</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="8">
-        <v>339</v>
-      </c>
-      <c r="J12" s="9">
-        <f>I12/$I$14</f>
-        <v>0.16560820713238886</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="8">
-        <v>491</v>
-      </c>
-      <c r="C13" s="9">
-        <f>B13/$B$14</f>
-        <v>0.18669201520912548</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="8">
-        <v>334</v>
-      </c>
-      <c r="J13" s="9">
-        <f>I13/$I$14</f>
-        <v>0.16316560820713238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <f>SUM(B8:B13)</f>
         <v>2630</v>
       </c>
-      <c r="C14" s="9">
-        <f>B14/$B$14</f>
+      <c r="C14" s="8">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" s="8">
+      <c r="H14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="7">
         <f>SUM(I8:I13)</f>
-        <v>2047</v>
-      </c>
-      <c r="J14" s="9">
-        <f>I14/$I$14</f>
+        <v>2093</v>
+      </c>
+      <c r="J14" s="8">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="4:4" ht="15">
-      <c r="D20" s="11"/>
+      <c r="D20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
FIX SYSTEM CONTENT IN api.py
</commit_message>
<xml_diff>
--- a/SimulationManager/Training LLM/TrainingStats.xlsx
+++ b/SimulationManager/Training LLM/TrainingStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\UnityProjects\SimulationManager\Training LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FAE153-8875-449E-ACAB-F0E511A51246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A42F376-498A-48BD-8F8E-2B5488B0F0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21FFF4A9-BEE3-4716-82C1-DB13693BAF4B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>MODELO</t>
   </si>
@@ -60,15 +60,6 @@
     <t>CHECKPOINTS</t>
   </si>
   <si>
-    <t>STEP-80</t>
-  </si>
-  <si>
-    <t>STEP-90</t>
-  </si>
-  <si>
-    <t>STEP-100</t>
-  </si>
-  <si>
     <t>TRAINED TOKENS</t>
   </si>
   <si>
@@ -202,6 +193,33 @@
   </si>
   <si>
     <t>*TODO CONSIDERANDO UNA LINEA DE JSONL PROMEDIO</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv4:B346BIAP</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv4:B346B2Fp:ckpt-step-12</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv4:B346Az6s:ckpt-step-8</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv5:B34rzjN4:ckpt-step-70</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv5:B34rzxJo:ckpt-step-84</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv5:B34s0MaY</t>
   </si>
 </sst>
 </file>
@@ -213,7 +231,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0;[Red]&quot;$&quot;\-#,##0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0000;[Red]&quot;$&quot;\-#,##0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +251,14 @@
       <color rgb="FFCE9178"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -271,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -301,9 +327,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,57 +672,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6976085A-B9FC-4CD1-931F-2113AEA9B965}">
-  <dimension ref="B3:Q11"/>
+  <dimension ref="B2:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:17">
-      <c r="B3" s="10" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="O3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="10" t="s">
+      <c r="P3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="Q3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
@@ -703,28 +741,28 @@
         <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="2:17" ht="28.5" customHeight="1">
+        <v>58</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2">
         <v>0.3</v>
@@ -739,13 +777,13 @@
         <v>3</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K5" s="3">
         <v>372550</v>
@@ -767,16 +805,16 @@
         <v>1.11765</v>
       </c>
       <c r="Q5" s="5">
-        <f>P5*996</f>
-        <v>1113.1794</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" ht="28.5" customHeight="1">
+        <f>P5*$Q$2</f>
+        <v>1052.8262999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2">
         <v>0.3</v>
@@ -791,13 +829,13 @@
         <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K6" s="3">
         <v>368950</v>
@@ -819,16 +857,16 @@
         <v>1.1068500000000001</v>
       </c>
       <c r="Q6" s="5">
-        <f t="shared" ref="Q6:Q10" si="1">P6*996</f>
-        <v>1102.4226000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="28.5" customHeight="1">
+        <f t="shared" ref="Q6:Q10" si="1">P6*$Q$2</f>
+        <v>1042.6527000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>0.3</v>
@@ -843,13 +881,13 @@
         <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K7" s="3">
         <v>328050</v>
@@ -872,15 +910,15 @@
       </c>
       <c r="Q7" s="5">
         <f t="shared" si="1"/>
-        <v>980.21340000000009</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" ht="28.5">
+        <v>927.06930000000011</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2">
         <v>0.3</v>
@@ -894,35 +932,45 @@
       <c r="G8" s="2">
         <v>3</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3"/>
+      <c r="H8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="3">
+        <v>143632</v>
+      </c>
       <c r="L8" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M8" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="N8" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="O8" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1937114649</v>
+      </c>
       <c r="P8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.43089600000000006</v>
       </c>
       <c r="Q8" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="28.5">
+        <v>405.90403200000003</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2">
         <v>0.3</v>
@@ -936,35 +984,45 @@
       <c r="G9" s="2">
         <v>3</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="1">
-        <v>10</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="H9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="3">
+        <v>251356</v>
+      </c>
+      <c r="L9" s="11">
+        <v>7</v>
+      </c>
+      <c r="M9" s="11">
         <v>1</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="11">
         <v>1.8</v>
       </c>
-      <c r="O9" s="1"/>
+      <c r="O9" s="1">
+        <v>2044383751</v>
+      </c>
       <c r="P9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75406800000000007</v>
       </c>
       <c r="Q9" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" ht="28.5">
+        <v>710.33205600000008</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2">
         <v>0.3</v>
@@ -982,15 +1040,9 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="1">
-        <v>10</v>
-      </c>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1.8</v>
-      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="4">
         <f t="shared" si="0"/>
@@ -1001,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1018,12 +1070,15 @@
       <c r="O11" s="1"/>
       <c r="P11" s="4">
         <f>SUM(P5:P10)</f>
-        <v>3.20865</v>
+        <v>4.3936140000000004</v>
       </c>
       <c r="Q11" s="4">
         <f>SUM(Q5:Q10)</f>
-        <v>3195.8154</v>
-      </c>
+        <v>4138.784388</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="L12" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1052,70 +1107,70 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="11" style="6"/>
-    <col min="4" max="4" width="14.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" style="6"/>
-    <col min="7" max="7" width="14.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11" style="6"/>
-    <col min="10" max="10" width="18.5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="D3" s="13"/>
+      <c r="H3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="H3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="J3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:13">
+        <v>45</v>
+      </c>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>439</v>
       </c>
@@ -1145,41 +1200,41 @@
         <v>2685</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" s="7">
         <v>616</v>
@@ -1189,7 +1244,7 @@
         <v>0.23422053231939163</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I8" s="7">
         <v>476</v>
@@ -1199,9 +1254,9 @@
         <v>0.22742474916387959</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" s="7">
         <v>843</v>
@@ -1211,7 +1266,7 @@
         <v>0.32053231939163496</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I9" s="7">
         <v>766</v>
@@ -1221,9 +1276,9 @@
         <v>0.36598184424271379</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" s="7">
         <v>87</v>
@@ -1233,7 +1288,7 @@
         <v>3.3079847908745248E-2</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I10" s="7">
         <v>78</v>
@@ -1243,9 +1298,9 @@
         <v>3.7267080745341616E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" s="7">
         <v>95</v>
@@ -1255,7 +1310,7 @@
         <v>3.6121673003802278E-2</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I11" s="7">
         <v>86</v>
@@ -1265,9 +1320,9 @@
         <v>4.1089345437171527E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B12" s="7">
         <v>498</v>
@@ -1277,7 +1332,7 @@
         <v>0.18935361216730037</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I12" s="7">
         <v>346</v>
@@ -1287,9 +1342,9 @@
         <v>0.16531294792164358</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13" s="7">
         <v>491</v>
@@ -1299,7 +1354,7 @@
         <v>0.18669201520912548</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I13" s="7">
         <v>341</v>
@@ -1309,9 +1364,9 @@
         <v>0.16292403248924989</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="7">
         <f>SUM(B8:B13)</f>
@@ -1322,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I14" s="7">
         <f>SUM(I8:I13)</f>
@@ -1333,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="4:4" ht="15">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FINETUNING V6 ALL OK
</commit_message>
<xml_diff>
--- a/SimulationManager/Training LLM/TrainingStats.xlsx
+++ b/SimulationManager/Training LLM/TrainingStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\UnityProjects\SimulationManager\Training LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A42F376-498A-48BD-8F8E-2B5488B0F0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6321B440-9E18-4F11-9805-5B8568EFC216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21FFF4A9-BEE3-4716-82C1-DB13693BAF4B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>MODELO</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv5:B34s0MaY</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv6:B4Y49YIK:ckpt-step-70</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv6:B4Y493eN:ckpt-step-84</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-llmv6:B4Y4AFah</t>
   </si>
 </sst>
 </file>
@@ -297,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -333,10 +342,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,7 +690,7 @@
   <dimension ref="B2:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,48 +701,48 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
@@ -749,13 +764,13 @@
       <c r="J4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
     </row>
     <row r="5" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -1036,21 +1051,37 @@
       <c r="G10" s="2">
         <v>3</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="H10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="3">
+        <v>250663</v>
+      </c>
+      <c r="L10" s="12">
+        <v>7</v>
+      </c>
+      <c r="M10" s="12">
+        <v>1</v>
+      </c>
+      <c r="N10" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="O10" s="1">
+        <v>191679768</v>
+      </c>
       <c r="P10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75198900000000002</v>
       </c>
       <c r="Q10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>708.37363800000003</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
@@ -1070,29 +1101,29 @@
       <c r="O11" s="1"/>
       <c r="P11" s="4">
         <f>SUM(P5:P10)</f>
-        <v>4.3936140000000004</v>
+        <v>5.1456030000000004</v>
       </c>
       <c r="Q11" s="4">
         <f>SUM(Q5:Q10)</f>
-        <v>4138.784388</v>
+        <v>4847.1580260000001</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L12" s="14"/>
+      <c r="L12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:K4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1129,7 +1160,7 @@
       <c r="C2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="15" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -1141,7 +1172,7 @@
       <c r="J2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="15" t="s">
         <v>31</v>
       </c>
       <c r="M2" s="6" t="s">
@@ -1158,7 +1189,7 @@
       <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="15"/>
       <c r="H3" s="7" t="s">
         <v>44</v>
       </c>
@@ -1168,7 +1199,7 @@
       <c r="J3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="13"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7">

</xml_diff>

<commit_message>
Unity Simulation Manager V1.0 + Executable
</commit_message>
<xml_diff>
--- a/SimulationManager/Training LLM/TrainingStats.xlsx
+++ b/SimulationManager/Training LLM/TrainingStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\UnityProjects\SimulationManager\Training LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62125EAF-29E4-4C7D-953A-DC69D0C06A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6246B719-284C-4E88-86BE-7B8A6E4EAFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="98">
   <si>
     <t>SYSTEM</t>
   </si>
@@ -268,6 +268,66 @@
   </si>
   <si>
     <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv2:BGXpqDtb</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv3:BI4DnCKj:ckpt-step-42</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv3:BI4Dnn4Y:ckpt-step-63</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv3:BI4DnNKm</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-23</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv3:BI4DnCKj:ckpt-step-43</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv3:BI4Dnn4Y:ckpt-step-64</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-24</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-25</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-26</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-27</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-28</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-29</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-30</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-31</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-32</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-33</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini-2024-07-34</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv4:BI4OYMzE:ckpt-step-46</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv4:BI4OZAh1:ckpt-step-69</t>
+  </si>
+  <si>
+    <t>ft:gpt-4o-mini-2024-07-18:personal:dots-2nd-llmv4:BI4OZWOZ</t>
   </si>
 </sst>
 </file>
@@ -301,11 +361,10 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -491,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -517,15 +576,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="7" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -547,9 +597,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="7" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -586,9 +633,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -596,6 +640,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="7" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -646,7 +693,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -954,632 +1001,1097 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:Q16"/>
+  <dimension ref="B1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q2" s="16">
+      <c r="Q2" s="13">
         <v>933</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="51" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="43" t="s">
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="45" t="s">
+      <c r="N3" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="47" t="s">
+      <c r="P3" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="41" t="s">
+      <c r="Q3" s="37" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="50"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="39" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="40" t="s">
+      <c r="J4" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="42"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="38"/>
     </row>
     <row r="5" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30">
+      <c r="B5" s="26">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="20">
         <v>0.3</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="20">
         <v>0.15</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="20">
         <v>1.2</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="20">
         <v>3</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="22">
         <v>372550</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="22">
         <v>10</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="22">
         <v>1</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="23">
         <v>1.8</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="24">
         <v>1159080520</v>
       </c>
-      <c r="P5" s="29">
+      <c r="P5" s="25">
         <f t="shared" ref="P5:P14" si="0">G5*(K5/1000000)</f>
         <v>1.11765</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="27">
         <f t="shared" ref="Q5:Q14" si="1">P5*$Q$2</f>
         <v>1042.7674500000001</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30">
+      <c r="B6" s="26">
         <v>2</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="20">
         <v>0.3</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="20">
         <v>0.15</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="20">
         <v>1.2</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="20">
         <v>3</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="22">
         <v>368950</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="22">
         <v>10</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="22">
         <v>1</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="23">
         <v>1.8</v>
       </c>
-      <c r="O6" s="28">
+      <c r="O6" s="24">
         <v>2000676016</v>
       </c>
-      <c r="P6" s="29">
+      <c r="P6" s="25">
         <f t="shared" si="0"/>
         <v>1.1068500000000001</v>
       </c>
-      <c r="Q6" s="31">
+      <c r="Q6" s="27">
         <f t="shared" si="1"/>
         <v>1032.6910500000001</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="30">
+      <c r="B7" s="26">
         <v>3</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="20">
         <v>0.3</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="20">
         <v>0.15</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="20">
         <v>1.2</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="20">
         <v>3</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="22">
         <v>328050</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="22">
         <v>10</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="22">
         <v>1</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="23">
         <v>1.8</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O7" s="24">
         <v>1111156053</v>
       </c>
-      <c r="P7" s="29">
+      <c r="P7" s="25">
         <f t="shared" si="0"/>
         <v>0.98415000000000008</v>
       </c>
-      <c r="Q7" s="31">
+      <c r="Q7" s="27">
         <f t="shared" si="1"/>
         <v>918.21195000000012</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="30">
+    <row r="8" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="20">
         <v>0.3</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="20">
         <v>0.15</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="20">
         <v>1.2</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="20">
         <v>3</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="22">
         <v>143632</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="22">
         <v>4</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="23">
         <v>0.1</v>
       </c>
-      <c r="N8" s="26">
+      <c r="N8" s="22">
         <v>4</v>
       </c>
-      <c r="O8" s="28">
+      <c r="O8" s="24">
         <v>1937114649</v>
       </c>
-      <c r="P8" s="29">
+      <c r="P8" s="25">
         <f t="shared" si="0"/>
         <v>0.43089600000000006</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="27">
         <f t="shared" si="1"/>
         <v>402.02596800000003</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30">
+    <row r="9" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="26">
         <v>5</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="20">
         <v>0.3</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="20">
         <v>0.15</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="20">
         <v>1.2</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="20">
         <v>3</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="22">
         <v>251356</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="22">
         <v>7</v>
       </c>
-      <c r="M9" s="26">
+      <c r="M9" s="22">
         <v>1</v>
       </c>
-      <c r="N9" s="27">
+      <c r="N9" s="23">
         <v>1.8</v>
       </c>
-      <c r="O9" s="28">
+      <c r="O9" s="24">
         <v>2044383751</v>
       </c>
-      <c r="P9" s="29">
+      <c r="P9" s="25">
         <f t="shared" si="0"/>
         <v>0.75406800000000007</v>
       </c>
-      <c r="Q9" s="31">
+      <c r="Q9" s="27">
         <f t="shared" si="1"/>
         <v>703.54544400000009</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="30">
+    <row r="10" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="26">
         <v>6</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="20">
         <v>0.3</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="20">
         <v>0.15</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="20">
         <v>1.2</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="20">
         <v>3</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="22">
         <v>250663</v>
       </c>
-      <c r="L10" s="26">
+      <c r="L10" s="22">
         <v>7</v>
       </c>
-      <c r="M10" s="26">
+      <c r="M10" s="22">
         <v>1</v>
       </c>
-      <c r="N10" s="27">
+      <c r="N10" s="23">
         <v>1.8</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="24">
         <v>191679768</v>
       </c>
-      <c r="P10" s="29">
+      <c r="P10" s="25">
         <f t="shared" si="0"/>
         <v>0.75198900000000002</v>
       </c>
-      <c r="Q10" s="31">
+      <c r="Q10" s="27">
         <f t="shared" si="1"/>
         <v>701.60573699999998</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="30">
+    <row r="11" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26">
         <v>7</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="20">
         <v>0.3</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="20">
         <v>0.15</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="20">
         <v>1.2</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="20">
         <v>3</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="22">
         <v>33290</v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="22">
         <v>5</v>
       </c>
-      <c r="M11" s="26">
+      <c r="M11" s="22">
         <v>1</v>
       </c>
-      <c r="N11" s="27">
+      <c r="N11" s="23">
         <v>1.8</v>
       </c>
-      <c r="O11" s="28">
+      <c r="O11" s="24">
         <v>1815509151</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11" s="25">
         <f t="shared" si="0"/>
         <v>9.987E-2</v>
       </c>
-      <c r="Q11" s="31">
+      <c r="Q11" s="27">
         <f t="shared" si="1"/>
         <v>93.178709999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="30">
+    <row r="12" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="26">
         <v>8</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="20">
         <v>0.3</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="20">
         <v>0.15</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="20">
         <v>1.2</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="20">
         <v>3</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="J12" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="22">
         <v>261810</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="22">
         <v>10</v>
       </c>
-      <c r="M12" s="26">
+      <c r="M12" s="22">
         <v>1</v>
       </c>
-      <c r="N12" s="27">
+      <c r="N12" s="23">
         <v>1.8</v>
       </c>
-      <c r="O12" s="28">
+      <c r="O12" s="24">
         <v>1875054926</v>
       </c>
-      <c r="P12" s="29">
+      <c r="P12" s="25">
         <f t="shared" si="0"/>
         <v>0.78542999999999996</v>
       </c>
-      <c r="Q12" s="31">
+      <c r="Q12" s="27">
         <f t="shared" si="1"/>
         <v>732.80619000000002</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="30">
+    <row r="13" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="26">
         <v>9</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="20">
         <v>0.3</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="20">
         <v>0.15</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="20">
         <v>1.2</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="20">
         <v>3</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="22">
         <v>27784</v>
       </c>
-      <c r="L13" s="26">
+      <c r="L13" s="22">
         <v>4</v>
       </c>
-      <c r="M13" s="26">
+      <c r="M13" s="22">
         <v>1</v>
       </c>
-      <c r="N13" s="27">
+      <c r="N13" s="23">
         <v>1.8</v>
       </c>
-      <c r="O13" s="28">
-        <v>1146409416</v>
-      </c>
-      <c r="P13" s="29">
+      <c r="O13" s="24">
+        <v>1815509151</v>
+      </c>
+      <c r="P13" s="25">
         <f t="shared" si="0"/>
         <v>8.3351999999999996E-2</v>
       </c>
-      <c r="Q13" s="31">
+      <c r="Q13" s="27">
         <f t="shared" si="1"/>
         <v>77.767415999999997</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="32"/>
-      <c r="C14" s="33" t="s">
+    <row r="14" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="26">
+        <v>10</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="20">
         <v>0.3</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="20">
         <v>0.15</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="20">
         <v>1.2</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="20">
         <v>3</v>
       </c>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="37">
+      <c r="H14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="22">
+        <v>27784</v>
+      </c>
+      <c r="L14" s="22">
+        <v>4</v>
+      </c>
+      <c r="M14" s="22">
+        <v>1</v>
+      </c>
+      <c r="N14" s="23">
+        <v>1.8</v>
+      </c>
+      <c r="O14" s="24">
+        <v>1146409416</v>
+      </c>
+      <c r="P14" s="25">
         <f t="shared" si="0"/>
+        <v>8.3351999999999996E-2</v>
+      </c>
+      <c r="Q14" s="27">
+        <f t="shared" si="1"/>
+        <v>77.767415999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26">
+        <v>11</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E15" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F15" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G15" s="20">
+        <v>3</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="22">
+        <v>27784</v>
+      </c>
+      <c r="L15" s="22">
+        <v>4</v>
+      </c>
+      <c r="M15" s="22">
+        <v>1</v>
+      </c>
+      <c r="N15" s="23">
+        <v>1.8</v>
+      </c>
+      <c r="O15" s="24">
+        <v>1540181535</v>
+      </c>
+      <c r="P15" s="25">
+        <f t="shared" ref="P15:P26" si="2">G15*(K15/1000000)</f>
+        <v>8.3351999999999996E-2</v>
+      </c>
+      <c r="Q15" s="27">
+        <f t="shared" ref="Q15:Q26" si="3">P15*$Q$2</f>
+        <v>77.767415999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="26">
+        <v>12</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F16" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G16" s="20">
+        <v>3</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="22">
+        <v>30096</v>
+      </c>
+      <c r="L16" s="22">
+        <v>4</v>
+      </c>
+      <c r="M16" s="22">
+        <v>1</v>
+      </c>
+      <c r="N16" s="23">
+        <v>1.8</v>
+      </c>
+      <c r="O16" s="24">
+        <v>2066556991</v>
+      </c>
+      <c r="P16" s="25">
+        <f t="shared" si="2"/>
+        <v>9.0288000000000007E-2</v>
+      </c>
+      <c r="Q16" s="27">
+        <f t="shared" si="3"/>
+        <v>84.238704000000013</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="26">
+        <v>13</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E17" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F17" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G17" s="20">
+        <v>3</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="25">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="38">
-        <f t="shared" si="1"/>
+      <c r="Q17" s="27">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="17">
-        <f>SUM(P5:P14)</f>
-        <v>6.114255</v>
-      </c>
-      <c r="Q15" s="17">
-        <f>SUM(Q5:Q14)</f>
-        <v>5704.5999150000007</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L16" s="23"/>
+    <row r="18" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="26">
+        <v>14</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G18" s="20">
+        <v>3</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26">
+        <v>15</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F19" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G19" s="20">
+        <v>3</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="26">
+        <v>16</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F20" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G20" s="20">
+        <v>3</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="26">
+        <v>17</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F21" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G21" s="20">
+        <v>3</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="26">
+        <v>18</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F22" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G22" s="20">
+        <v>3</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26">
+        <v>19</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F23" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G23" s="20">
+        <v>3</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26">
+        <v>20</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E24" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F24" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G24" s="20">
+        <v>3</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="26">
+        <v>21</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E25" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F25" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="G25" s="20">
+        <v>3</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="28">
+        <v>22</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0.15</v>
+      </c>
+      <c r="F26" s="30">
+        <v>1.2</v>
+      </c>
+      <c r="G26" s="30">
+        <v>3</v>
+      </c>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="14">
+        <f>SUM(P5:P26)</f>
+        <v>6.3712469999999994</v>
+      </c>
+      <c r="Q27" s="14">
+        <f>SUM(Q5:Q26)</f>
+        <v>5944.3734510000004</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1595,7 +2107,9 @@
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1646,7 +2160,7 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="50" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3"/>
@@ -1661,7 +2175,7 @@
       <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="50" t="s">
         <v>3</v>
       </c>
       <c r="L2" s="3"/>
@@ -1679,7 +2193,7 @@
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1692,7 +2206,7 @@
       <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="55"/>
+      <c r="K3" s="51"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>

</xml_diff>